<commit_message>
Update notebook and excel
</commit_message>
<xml_diff>
--- a/dnd.xlsx
+++ b/dnd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay Colond\dnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D51CF7C-C451-433D-BE1E-4A1B832F7C83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BC56EC-A1BA-48AA-8626-7CB1877D34C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -958,7 +958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1336,7 +1338,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
restored dnd prep for next draft
</commit_message>
<xml_diff>
--- a/dnd.xlsx
+++ b/dnd.xlsx
@@ -5,26 +5,43 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay Colond\dnd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af61fef4f68a2aa9/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8B4D03-AFE8-4F30-9F7D-EA2D6E0D5383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7300DFEB-F2AB-4E32-A276-0777BC5F4F44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AGIEFC" sheetId="1" r:id="rId1"/>
+    <sheet name="AGI" sheetId="1" r:id="rId1"/>
+    <sheet name="EFC" sheetId="2" r:id="rId2"/>
+    <sheet name="Help" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="31">
+  <si>
+    <t>SE_Bigger_50</t>
+  </si>
   <si>
     <t>100-30000</t>
   </si>
   <si>
+    <t xml:space="preserve">  White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Black or African American</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hispanic or Latino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Asian</t>
+  </si>
+  <si>
     <t>30001-48000</t>
   </si>
   <si>
@@ -49,6 +66,30 @@
     <t>$15,600 or more</t>
   </si>
   <si>
+    <t>No help</t>
+  </si>
+  <si>
+    <t>Tuition only</t>
+  </si>
+  <si>
+    <t>Nontuition only</t>
+  </si>
+  <si>
+    <t>Tuition and nontuition</t>
+  </si>
+  <si>
+    <t>Independent student</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
     <t>Asian</t>
   </si>
   <si>
@@ -58,34 +99,22 @@
     <t>Race_Ethnicity</t>
   </si>
   <si>
+    <t>Debt_ratio</t>
+  </si>
+  <si>
     <t>EFC</t>
   </si>
   <si>
+    <t>Parent_help</t>
+  </si>
+  <si>
     <t>AGI_Label</t>
   </si>
   <si>
     <t>EFC_Label</t>
   </si>
   <si>
-    <t>Debt_ratio_AGI</t>
-  </si>
-  <si>
-    <t>SE_Bigger_50_AGI</t>
-  </si>
-  <si>
-    <t>Debt_ratio_EFC</t>
-  </si>
-  <si>
-    <t>SE_Bigger_50_EFC</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Latinx</t>
+    <t>Parent_help_Label</t>
   </si>
 </sst>
 </file>
@@ -927,89 +956,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -1021,15 +1038,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1">
         <v>24</v>
@@ -1038,46 +1055,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>110</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="1">
-        <v>57</v>
-      </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -1089,15 +1106,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1">
         <v>45</v>
@@ -1106,46 +1123,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1">
+        <v>57.595599999999997</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>96.126300000000001</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1">
-        <v>57.595599999999997</v>
-      </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -1157,15 +1174,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1">
         <v>50.4191</v>
@@ -1174,46 +1191,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>113</v>
       </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1">
-        <v>58</v>
-      </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
@@ -1225,15 +1242,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1">
         <v>30</v>
@@ -1242,46 +1259,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -1293,360 +1310,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D21" s="1">
         <v>47</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>105</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>89</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>69</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>25</v>
-      </c>
-      <c r="I25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="1">
-        <v>106</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="1">
-        <v>67</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-      <c r="G28" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="1">
-        <v>87</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-      <c r="G29" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="1">
-        <v>60</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30">
-        <v>3</v>
-      </c>
-      <c r="G30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="1">
-        <v>104</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
-      <c r="G31" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="1">
-        <v>65</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32">
-        <v>3</v>
-      </c>
-      <c r="G32" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="1">
-        <v>87</v>
-      </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33">
-        <v>3</v>
-      </c>
-      <c r="G33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="1">
-        <v>33</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34">
-        <v>4</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="1">
-        <v>105</v>
-      </c>
-      <c r="I34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="1">
-        <v>55</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36">
-        <v>4</v>
-      </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="1">
-        <v>89</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37">
-        <v>4</v>
-      </c>
-      <c r="G37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="1">
-        <v>47</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38">
-        <v>5</v>
-      </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="1">
-        <v>108</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39">
-        <v>5</v>
-      </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="1">
-        <v>49</v>
-      </c>
-      <c r="I39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40">
-        <v>5</v>
-      </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="1">
-        <v>80</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41">
-        <v>5</v>
-      </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="1">
-        <v>47</v>
-      </c>
-      <c r="I41" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1654,4 +1331,682 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>89</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>105</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>106</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>87</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>65</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>104</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>87</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>105</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>89</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>108</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>80</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>71</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>104</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>80</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>51</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>97</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>77</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>107</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>87</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>107</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>83</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>93</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>104</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>75</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>